<commit_message>
first round of 3.3 files
</commit_message>
<xml_diff>
--- a/InputData/bldgs/RBFF/Recipient Buildings Fuel Fractions.xlsx
+++ b/InputData/bldgs/RBFF/Recipient Buildings Fuel Fractions.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Documents\EPS_Models by Region\RMI\All_states_RMI\template_state\bldgs\RBFF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Documents\EPS_Models by Region\United States\NEW_US\InputData\bldgs\RBFF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57B018FF-DE0F-4CED-887E-09249D95ED5E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE4E3257-D795-4A92-804F-0180AA3862CC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9660" yWindow="1080" windowWidth="17205" windowHeight="16065" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -135,7 +135,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -151,7 +151,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -432,7 +431,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J13" sqref="J13"/>
@@ -440,15 +439,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="7">
-        <v>44316</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -456,42 +452,42 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>21</v>
       </c>

</xml_diff>